<commit_message>
data is incorrect, but fixed a problem where instrctions are squashed by squashes
</commit_message>
<xml_diff>
--- a/cpu_data.xlsx
+++ b/cpu_data.xlsx
@@ -63,10 +63,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,13 +105,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -374,7 +394,7 @@
   <dimension ref="B2:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,8 +504,109 @@
       <c r="B9" t="s">
         <v>10</v>
       </c>
+      <c r="D9">
+        <v>182819906</v>
+      </c>
+      <c r="E9">
+        <v>177151873</v>
+      </c>
+      <c r="F9">
+        <v>177683557</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A9:XFD9">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:XFD8">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:XFD7">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:XFD6">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:XFD5">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:XFD4">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:XFD3">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed results, baselines for samples 0-4
</commit_message>
<xml_diff>
--- a/cpu_data.xlsx
+++ b/cpu_data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Devon/Documents/git/7cyclesim/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MCI10\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="21600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -123,6 +123,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -390,19 +393,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -416,102 +419,54 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="D3">
-        <v>1580</v>
-      </c>
-      <c r="E3">
-        <v>1583</v>
-      </c>
-      <c r="F3">
-        <v>1578</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="D4">
-        <v>1968190</v>
-      </c>
-      <c r="E4">
-        <v>1844314</v>
-      </c>
-      <c r="F4">
-        <v>1844612</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+        <v>2036448</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="D5">
-        <v>1808609</v>
-      </c>
-      <c r="E5">
-        <v>1791784</v>
-      </c>
-      <c r="F5">
-        <v>1783558</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+        <v>1905766</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="D6">
-        <v>1974558</v>
-      </c>
-      <c r="E6">
-        <v>1962910</v>
-      </c>
-      <c r="F6">
-        <v>1969840</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+        <v>2115927</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="D7">
-        <v>5751348</v>
-      </c>
-      <c r="E7">
-        <v>5599001</v>
-      </c>
-      <c r="F7">
-        <v>5598003</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+        <v>6058130</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="D8">
-        <v>171167356</v>
-      </c>
-      <c r="E8">
-        <v>165883247</v>
-      </c>
-      <c r="F8">
-        <v>165551910</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>10</v>
-      </c>
-      <c r="D9">
-        <v>182819906</v>
-      </c>
-      <c r="E9">
-        <v>177151873</v>
-      </c>
-      <c r="F9">
-        <v>177683557</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data is in the deliverable folder
</commit_message>
<xml_diff>
--- a/cpu_data.xlsx
+++ b/cpu_data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MCI10\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Devon/Documents/git/7cyclesim/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="9040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>bp - 0</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>bp - 1</t>
   </si>
@@ -57,12 +54,42 @@
   </si>
   <si>
     <t>sample_large2.tr</t>
+  </si>
+  <si>
+    <t>Prediction Method - 1</t>
+  </si>
+  <si>
+    <t>Prediction Method - 0</t>
+  </si>
+  <si>
+    <t>Prediction Method - 2</t>
+  </si>
+  <si>
+    <t>Percent Improvement: (Method 0 - Method 1) / Method 0</t>
+  </si>
+  <si>
+    <t>Percent Improvement: (Method 0 - Method 2) / Method 0</t>
+  </si>
+  <si>
+    <t>32 bit</t>
+  </si>
+  <si>
+    <t>128 bit</t>
+  </si>
+  <si>
+    <t>64 bit</t>
+  </si>
+  <si>
+    <t>Percent Improvement: (32 bit - 64 bit) / 32 bit</t>
+  </si>
+  <si>
+    <t>Percent Improvement: (32 bit - 128 bit) / 32 bit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -105,17 +132,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -393,85 +439,435 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.796875" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" style="1"/>
+    <col min="2" max="2" width="21.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="1"/>
+    <col min="4" max="4" width="19.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.1640625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+    <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" s="1">
+        <v>1625</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1633</v>
+      </c>
+      <c r="F3" s="1">
+        <f>(D3-E3)/D3*100</f>
+        <v>-0.49230769230769234</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1628</v>
+      </c>
+      <c r="H3" s="1">
+        <f>(D3-G3)/D3*100</f>
+        <v>-0.1846153846153846</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2036448</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1930650</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F9" si="0">(D4-E4)/D4*100</f>
+        <v>5.1952222693631267</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1931267</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" ref="H4:H9" si="1">(D4-G4)/D4*100</f>
+        <v>5.1649244174169926</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1905766</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1875057</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6113730646889493</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1867550</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="1"/>
+        <v>2.005282915111299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2115927</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2102172</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.65006968576893254</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2088474</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="1"/>
+        <v>1.2974455167876775</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6058130</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5907871</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4802868211807936</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5887283</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="1"/>
+        <v>2.8201276631567826</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1">
+        <v>179428164</v>
+      </c>
+      <c r="E8" s="1">
+        <v>173558171</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>3.2715003426106506</v>
+      </c>
+      <c r="G8" s="1">
+        <v>171910134</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="1"/>
+        <v>4.1899943868343881</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1">
+        <v>194292230</v>
+      </c>
+      <c r="E9" s="1">
+        <v>190081856</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>2.167031589477356</v>
+      </c>
+      <c r="G9" s="1">
+        <v>189016538</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="1"/>
+        <v>2.7153386422092125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1633</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1633</v>
+      </c>
+      <c r="F12" s="1">
+        <f>(D12-E12)/D12*100</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1633</v>
+      </c>
+      <c r="H12" s="1">
+        <f>(D12-G12)/D12*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1">
+        <v>5910725</v>
+      </c>
+      <c r="E13" s="1">
+        <v>5907871</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" ref="F13:F15" si="2">(D13-E13)/D13*100</f>
+        <v>4.828510884874529E-2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>5902270</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" ref="H13:H15" si="3">(D13-G13)/D13*100</f>
+        <v>0.14304505792436631</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="1">
+        <v>173568792</v>
+      </c>
+      <c r="E14" s="1">
+        <v>173558171</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="2"/>
+        <v>6.1191876014208826E-3</v>
+      </c>
+      <c r="G14" s="1">
+        <v>172113225</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="3"/>
+        <v>0.83861101020971562</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="1">
+        <v>190087976</v>
+      </c>
+      <c r="E15" s="1">
+        <v>190081856</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="2"/>
+        <v>3.2195618727614839E-3</v>
+      </c>
+      <c r="G15" s="1">
+        <v>190084482</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="3"/>
+        <v>1.8380962718020628E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="B18" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>1625</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>2036448</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>1905766</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="D18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1628</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1628</v>
+      </c>
+      <c r="F19" s="1">
+        <f>(D19-E19)/D19*100</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1628</v>
+      </c>
+      <c r="H19" s="1">
+        <f>(D19-E19)/D19*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6">
-        <v>2115927</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="D20" s="1">
+        <v>5890986</v>
+      </c>
+      <c r="E20" s="1">
+        <v>5887283</v>
+      </c>
+      <c r="F20" s="1">
+        <f>(D20-E20)/D20*100</f>
+        <v>6.2858747245367746E-2</v>
+      </c>
+      <c r="G20" s="1">
+        <v>5879200</v>
+      </c>
+      <c r="H20" s="1">
+        <f>(D20-G20)/D20*100</f>
+        <v>0.20006837565052776</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D7">
-        <v>6058130</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="D21" s="1">
+        <v>171921878</v>
+      </c>
+      <c r="E21" s="1">
+        <v>171910134</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" ref="F21:F22" si="4">(D21-E21)/D21*100</f>
+        <v>6.8310096054208999E-3</v>
+      </c>
+      <c r="G21" s="1">
+        <v>170474636</v>
+      </c>
+      <c r="H21" s="1">
+        <f>(D21-G21)/D21*100</f>
+        <v>0.84180211200345301</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>10</v>
+      <c r="D22" s="1">
+        <v>189026296</v>
+      </c>
+      <c r="E22" s="1">
+        <v>189016538</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="4"/>
+        <v>5.162244728109151E-3</v>
+      </c>
+      <c r="G22" s="1">
+        <v>189022690</v>
+      </c>
+      <c r="H22" s="1">
+        <f>(D22-G22)/D22*100</f>
+        <v>1.9076710893176471E-3</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A9:XFD9">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="A9:E9 G9 I9:XFD9">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -479,30 +875,180 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8:XFD8">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7:XFD7">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:E8 G8 I8:XFD8">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:E7 G7 I7:XFD7">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:E6 G6 I6:XFD6">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:E5 G5 I5:XFD5">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:E4 G4 I4:XFD4">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:E3 G3">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:E15 G15">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:E14 G14">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:E13 G13">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:E12 G12">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22:E22">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21:E21">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:E20">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19:E19">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -514,7 +1060,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6:XFD6">
+  <conditionalFormatting sqref="D22:E22 G22">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -526,7 +1072,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:XFD5">
+  <conditionalFormatting sqref="D21:E21 G21">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -538,7 +1084,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:XFD4">
+  <conditionalFormatting sqref="D20:E20 E28 G20">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -550,7 +1096,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:XFD3">
+  <conditionalFormatting sqref="D19:E19 G19">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>